<commit_message>
Chapter 4 fixed exercises
</commit_message>
<xml_diff>
--- a/DataManipulationVisualisation/data/spruce_forest_wide_long/spruce_forestLONG.xlsx
+++ b/DataManipulationVisualisation/data/spruce_forest_wide_long/spruce_forestLONG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\IA\VYUKA\BotzoolDataAnalysis\DataManipulationVisualisation\data\spruce_forest_wide_long\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48454B7E-45FF-43BA-9904-5190686EB87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC495A6-3A46-4069-9860-87EFCF9AF7D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="22">
   <si>
     <t>sites</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Site6</t>
+  </si>
+  <si>
+    <t>layer</t>
   </si>
 </sst>
 </file>
@@ -477,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,7 +491,7 @@
     <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,8 +501,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -509,8 +515,11 @@
       <c r="C2" s="2">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -520,8 +529,11 @@
       <c r="C3" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -531,8 +543,11 @@
       <c r="C4" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -542,8 +557,11 @@
       <c r="C5" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -553,8 +571,11 @@
       <c r="C6" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -564,8 +585,11 @@
       <c r="C7" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -575,8 +599,11 @@
       <c r="C8" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -586,8 +613,11 @@
       <c r="C9" s="3">
         <v>85</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -597,8 +627,11 @@
       <c r="C10" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -608,8 +641,11 @@
       <c r="C11" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -619,8 +655,11 @@
       <c r="C12" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -630,8 +669,11 @@
       <c r="C13" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
@@ -641,8 +683,11 @@
       <c r="C14" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
@@ -652,8 +697,11 @@
       <c r="C15" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
@@ -663,8 +711,11 @@
       <c r="C16" s="4">
         <v>70</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
@@ -674,8 +725,11 @@
       <c r="C17" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>12</v>
       </c>
@@ -685,8 +739,11 @@
       <c r="C18" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
@@ -696,8 +753,11 @@
       <c r="C19" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>12</v>
       </c>
@@ -707,8 +767,11 @@
       <c r="C20" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>12</v>
       </c>
@@ -718,8 +781,11 @@
       <c r="C21" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>13</v>
       </c>
@@ -729,8 +795,11 @@
       <c r="C22" s="5">
         <v>65</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>13</v>
       </c>
@@ -740,8 +809,11 @@
       <c r="C23" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>13</v>
       </c>
@@ -751,8 +823,11 @@
       <c r="C24" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>13</v>
       </c>
@@ -762,8 +837,11 @@
       <c r="C25" s="5">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>13</v>
       </c>
@@ -773,8 +851,11 @@
       <c r="C26" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>13</v>
       </c>
@@ -784,8 +865,11 @@
       <c r="C27" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>13</v>
       </c>
@@ -795,8 +879,11 @@
       <c r="C28" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>13</v>
       </c>
@@ -806,8 +893,11 @@
       <c r="C29" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>19</v>
       </c>
@@ -817,8 +907,11 @@
       <c r="C30" s="6">
         <v>80</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>19</v>
       </c>
@@ -828,8 +921,11 @@
       <c r="C31" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>19</v>
       </c>
@@ -839,8 +935,11 @@
       <c r="C32" s="6">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>19</v>
       </c>
@@ -850,8 +949,11 @@
       <c r="C33" s="6">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>19</v>
       </c>
@@ -861,8 +963,11 @@
       <c r="C34" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>19</v>
       </c>
@@ -872,8 +977,11 @@
       <c r="C35" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>19</v>
       </c>
@@ -883,8 +991,11 @@
       <c r="C36" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>19</v>
       </c>
@@ -894,8 +1005,11 @@
       <c r="C37" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>20</v>
       </c>
@@ -905,8 +1019,11 @@
       <c r="C38" s="7">
         <v>65</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>20</v>
       </c>
@@ -916,8 +1033,11 @@
       <c r="C39" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>20</v>
       </c>
@@ -927,8 +1047,11 @@
       <c r="C40" s="7">
         <v>30</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>20</v>
       </c>
@@ -938,8 +1061,11 @@
       <c r="C41" s="7">
         <v>25</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>20</v>
       </c>
@@ -949,8 +1075,11 @@
       <c r="C42" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>20</v>
       </c>
@@ -960,8 +1089,11 @@
       <c r="C43" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>20</v>
       </c>
@@ -970,6 +1102,9 @@
       </c>
       <c r="C44" s="7">
         <v>1</v>
+      </c>
+      <c r="D44">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>